<commit_message>
inle 66 , 69
</commit_message>
<xml_diff>
--- a/inle_functions.xlsx
+++ b/inle_functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inle_bush/Desktop/solutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B328946-2974-B540-9465-BDE37078C640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C9D907-6C99-8441-B9A1-D15499B1EE5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="15080" windowHeight="13840" xr2:uid="{D1DFE109-4487-DB4B-8C3B-ED6D0B4F8677}"/>
   </bookViews>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA7269E-7790-E547-AC91-FA3CE9D40C51}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
folderize, inle 51, inle 1 v2
</commit_message>
<xml_diff>
--- a/inle_functions.xlsx
+++ b/inle_functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inle_bush/Desktop/cs/solutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A439C832-CD82-994E-844C-B87D31A10F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C11F905-9902-764D-A302-99A027B21866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9580" yWindow="3200" windowWidth="15080" windowHeight="13820" xr2:uid="{D1DFE109-4487-DB4B-8C3B-ED6D0B4F8677}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" xr2:uid="{D1DFE109-4487-DB4B-8C3B-ED6D0B4F8677}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -629,14 +629,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{380B3E3B-1E09-3F45-B483-A204D9C54BD4}" name="Table1" displayName="Table1" ref="A1:H55" totalsRowShown="0">
-  <autoFilter ref="A1:H55" xr:uid="{6328D835-E1DA-0A4B-9C1A-999543367B28}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="vector number , base"/>
-        <filter val="vector number , list number , string number, base"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H55" xr:uid="{6328D835-E1DA-0A4B-9C1A-999543367B28}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0A88C72C-048B-354A-B5C0-BBF537E1DD4E}" name="Number"/>
     <tableColumn id="2" xr3:uid="{3EAB488D-33C3-4F46-9237-E4489BF71D10}" name="Function Name"/>
@@ -950,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA7269E-7790-E547-AC91-FA3CE9D40C51}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,7 +982,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1012,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1035,7 +1028,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1058,7 +1051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1081,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1107,7 +1100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1130,7 +1123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1153,7 +1146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1176,7 +1169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1202,7 +1195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1225,7 +1218,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1248,7 +1241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1271,7 +1264,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1294,7 +1287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1317,7 +1310,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1343,7 +1336,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1363,7 +1356,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1435,7 +1428,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1461,7 +1454,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1484,7 +1477,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1504,7 +1497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1530,7 +1523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1553,7 +1546,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1576,7 +1569,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1622,7 +1615,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1645,7 +1638,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1668,7 +1661,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1691,7 +1684,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1714,7 +1707,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1737,7 +1730,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1760,7 +1753,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1783,7 +1776,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1806,7 +1799,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1829,7 +1822,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1852,7 +1845,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1875,7 +1868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1898,77 +1891,77 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>

</xml_diff>